<commit_message>
add train test comparison
</commit_message>
<xml_diff>
--- a/train_test_score_comparison.xlsx
+++ b/train_test_score_comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/jgrusy3_gatech_edu/Documents/OMSCS/CS7641-ML/SupervisedLearning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Grusy\OneDrive - Georgia Institute of Technology\OMSCS\CS7641-ML\SupervisedLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BB06BC9-B327-4B5F-8CD3-B44178A16CF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{6BB06BC9-B327-4B5F-8CD3-B44178A16CF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A3E90F73-0901-4029-92C9-8F72B7BF3654}"/>
   <bookViews>
-    <workbookView xWindow="28890" yWindow="2655" windowWidth="21600" windowHeight="11505" xr2:uid="{A5B969B2-372F-482A-A308-0C10F2D3024F}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{A5B969B2-372F-482A-A308-0C10F2D3024F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>Algorithm</t>
   </si>
@@ -187,6 +187,24 @@
   </si>
   <si>
     <t>ANN</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>RBF</t>
+  </si>
+  <si>
+    <t>Polynomial</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>Max Accuracy Score</t>
+  </si>
+  <si>
+    <t>Mean Train Time (s)</t>
   </si>
 </sst>
 </file>
@@ -381,20 +399,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -402,14 +414,21 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,7 +746,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,16 +779,16 @@
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="11">
         <v>1.25337829395216E-2</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="11">
         <v>1.7846010169204399E-3</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="14">
         <v>0.81770833333333304</v>
       </c>
       <c r="H2" t="s">
@@ -777,17 +796,17 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <v>5.6917700962144498E-2</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="13">
         <v>1.23968951556147E-3</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="15">
         <v>0.59162838182746302</v>
       </c>
       <c r="H3" t="s">
@@ -795,19 +814,19 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>4.0723284214973399</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>3.8722664833068798E-3</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>0.81462500000000004</v>
       </c>
       <c r="H4" t="s">
@@ -815,17 +834,17 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2.5873445343971202</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>2.01020097732543E-3</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>0.53956100051046396</v>
       </c>
       <c r="H5" t="s">
@@ -836,16 +855,16 @@
       <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>2.8604187520742399</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="11">
         <v>0.24175926142930901</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <v>0.81708333333333305</v>
       </c>
       <c r="H6" t="s">
@@ -853,17 +872,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="13">
         <v>1.3895188165307</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>8.5532168507576001E-2</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="15">
         <v>0.50995405819295503</v>
       </c>
       <c r="H7" t="s">
@@ -871,19 +890,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>102.058048921823</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.43943319916725099</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>0.81899999999999995</v>
       </c>
       <c r="H8" t="s">
@@ -891,17 +910,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>1.08491452932357</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.168332493305206</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>0.59622256253190398</v>
       </c>
       <c r="H9" t="s">
@@ -912,16 +931,16 @@
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>0.41469445824623102</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="11">
         <v>0.97940683364868097</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>0.83116666666666605</v>
       </c>
       <c r="H10" t="s">
@@ -929,17 +948,17 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <v>2.37207611401875E-3</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="8">
         <v>7.9322059949238993E-2</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="9">
         <v>0.52857142857142803</v>
       </c>
       <c r="H11" t="s">
@@ -956,97 +975,175 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="H15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.73880000000000001</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0.81899999999999995</v>
+      </c>
       <c r="H16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.45288</v>
+      </c>
+      <c r="D17" s="15">
+        <v>0.59599999999999997</v>
+      </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5">
+        <v>253.84200000000001</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.8075</v>
+      </c>
       <c r="H18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="5">
+        <v>5.1836000000000002</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.52500000000000002</v>
+      </c>
       <c r="H19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.77749999999999997</v>
+      </c>
       <c r="H20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19"/>
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.28039999999999998</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.501</v>
+      </c>
       <c r="H21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>41</v>
       </c>
@@ -1097,7 +1194,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
@@ -1109,6 +1209,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B1D9173FAF0D234D956856A51ABC1AB1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0abb02dfca027369b3877011dccae479">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="da2d671d-84db-436a-a5cf-17d7d30e5161" xmlns:ns4="cca7bc4e-1af1-47a1-b763-9d128f5b64ab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af1d68f730b2429c2be4e2d072b04957" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1348,15 +1457,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1367,6 +1467,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9510040-7C43-4C9F-A4A0-EA46308B83E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{746C2368-ACC5-4ABE-BB88-42B067742C22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1386,14 +1494,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9510040-7C43-4C9F-A4A0-EA46308B83E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C3240EF-595E-4207-9EF6-AC23790293E6}">
   <ds:schemaRefs>

</xml_diff>